<commit_message>
Added day of the week
</commit_message>
<xml_diff>
--- a/calc.xlsx
+++ b/calc.xlsx
@@ -1758,8 +1758,8 @@
   <dimension ref="A3:U50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31:XFD31"/>
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1791,6 +1791,28 @@
       </c>
       <c r="D4" s="32"/>
     </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="L6" s="5" t="str">
+        <f ca="1">TEXT(L7,"ддд")</f>
+        <v>Ср</v>
+      </c>
+      <c r="M6" s="5" t="str">
+        <f ca="1">TEXT(M7,"ддд")</f>
+        <v>Вт</v>
+      </c>
+      <c r="N6" s="5" t="str">
+        <f t="shared" ref="N6:P6" ca="1" si="0">TEXT(N7,"ддд")</f>
+        <v>Пн</v>
+      </c>
+      <c r="O6" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Пт</v>
+      </c>
+      <c r="P6" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Чт</v>
+      </c>
+    </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>31</v>
@@ -1861,7 +1883,7 @@
         <v>0.6</v>
       </c>
       <c r="D8" s="25">
-        <f t="shared" ref="D8:D25" si="0">C8/10</f>
+        <f t="shared" ref="D8:D25" si="1">C8/10</f>
         <v>0.06</v>
       </c>
       <c r="E8" s="22">
@@ -1871,11 +1893,11 @@
         <v>0.1</v>
       </c>
       <c r="G8" s="26">
-        <f t="shared" ref="G8:G25" si="1">ROUND($C$4/(D8/E8*F8),0)</f>
+        <f t="shared" ref="G8:G25" si="2">ROUND($C$4/(D8/E8*F8),0)</f>
         <v>336</v>
       </c>
       <c r="H8" s="22">
-        <f t="shared" ref="H8:H16" si="2">ROUND(D8/E8,0)</f>
+        <f t="shared" ref="H8:H16" si="3">ROUND(D8/E8,0)</f>
         <v>60</v>
       </c>
       <c r="I8" s="23"/>
@@ -1923,7 +1945,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
       <c r="E9" s="1">
@@ -1933,11 +1955,11 @@
         <v>0.1</v>
       </c>
       <c r="G9" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>672</v>
       </c>
       <c r="H9" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="I9" s="23"/>
@@ -1954,15 +1976,15 @@
         <v>1.4200000000000017</v>
       </c>
       <c r="N9">
-        <f t="shared" ref="N9:N47" ca="1" si="3">VALUE(SUBSTITUTE(_xlfn.FILTERXML(_xlfn.WEBSERVICE("https://iss.moex.com/iss/engines/stock/markets/shares/securities/"&amp;B9&amp;"/candles.xml?from="&amp;$N$7&amp;"&amp;till="&amp;$N$7&amp;"&amp;interval=24"),"//document//data//rows//row/@high"),".",","))-VALUE(SUBSTITUTE(_xlfn.FILTERXML(_xlfn.WEBSERVICE("https://iss.moex.com/iss/engines/stock/markets/shares/securities/"&amp;B9&amp;"/candles.xml?from="&amp;$N$7&amp;"&amp;till="&amp;$N$7&amp;"&amp;interval=24"),"//document//data//rows//row/@low"),".",","))</f>
+        <f t="shared" ref="N9:N47" ca="1" si="4">VALUE(SUBSTITUTE(_xlfn.FILTERXML(_xlfn.WEBSERVICE("https://iss.moex.com/iss/engines/stock/markets/shares/securities/"&amp;B9&amp;"/candles.xml?from="&amp;$N$7&amp;"&amp;till="&amp;$N$7&amp;"&amp;interval=24"),"//document//data//rows//row/@high"),".",","))-VALUE(SUBSTITUTE(_xlfn.FILTERXML(_xlfn.WEBSERVICE("https://iss.moex.com/iss/engines/stock/markets/shares/securities/"&amp;B9&amp;"/candles.xml?from="&amp;$N$7&amp;"&amp;till="&amp;$N$7&amp;"&amp;interval=24"),"//document//data//rows//row/@low"),".",","))</f>
         <v>1.009999999999998</v>
       </c>
       <c r="O9">
-        <f t="shared" ref="O9:O47" ca="1" si="4">VALUE(SUBSTITUTE(_xlfn.FILTERXML(_xlfn.WEBSERVICE("https://iss.moex.com/iss/engines/stock/markets/shares/securities/"&amp;B9&amp;"/candles.xml?from="&amp;$O$7&amp;"&amp;till="&amp;$O$7&amp;"&amp;interval=24"),"//document//data//rows//row/@high"),".",","))-VALUE(SUBSTITUTE(_xlfn.FILTERXML(_xlfn.WEBSERVICE("https://iss.moex.com/iss/engines/stock/markets/shares/securities/"&amp;B9&amp;"/candles.xml?from="&amp;$O$7&amp;"&amp;till="&amp;$O$7&amp;"&amp;interval=24"),"//document//data//rows//row/@low"),".",","))</f>
+        <f t="shared" ref="O9:O47" ca="1" si="5">VALUE(SUBSTITUTE(_xlfn.FILTERXML(_xlfn.WEBSERVICE("https://iss.moex.com/iss/engines/stock/markets/shares/securities/"&amp;B9&amp;"/candles.xml?from="&amp;$O$7&amp;"&amp;till="&amp;$O$7&amp;"&amp;interval=24"),"//document//data//rows//row/@high"),".",","))-VALUE(SUBSTITUTE(_xlfn.FILTERXML(_xlfn.WEBSERVICE("https://iss.moex.com/iss/engines/stock/markets/shares/securities/"&amp;B9&amp;"/candles.xml?from="&amp;$O$7&amp;"&amp;till="&amp;$O$7&amp;"&amp;interval=24"),"//document//data//rows//row/@low"),".",","))</f>
         <v>1.25</v>
       </c>
       <c r="P9">
-        <f t="shared" ref="P9:P47" ca="1" si="5">VALUE(SUBSTITUTE(_xlfn.FILTERXML(_xlfn.WEBSERVICE("https://iss.moex.com/iss/engines/stock/markets/shares/securities/"&amp;B9&amp;"/candles.xml?from="&amp;$P$7&amp;"&amp;till="&amp;$P$7&amp;"&amp;interval=24"),"//document//data//rows//row/@high"),".",","))-VALUE(SUBSTITUTE(_xlfn.FILTERXML(_xlfn.WEBSERVICE("https://iss.moex.com/iss/engines/stock/markets/shares/securities/"&amp;B9&amp;"/candles.xml?from="&amp;$P$7&amp;"&amp;till="&amp;$P$7&amp;"&amp;interval=24"),"//document//data//rows//row/@low"),".",","))</f>
+        <f t="shared" ref="P9:P47" ca="1" si="6">VALUE(SUBSTITUTE(_xlfn.FILTERXML(_xlfn.WEBSERVICE("https://iss.moex.com/iss/engines/stock/markets/shares/securities/"&amp;B9&amp;"/candles.xml?from="&amp;$P$7&amp;"&amp;till="&amp;$P$7&amp;"&amp;interval=24"),"//document//data//rows//row/@high"),".",","))-VALUE(SUBSTITUTE(_xlfn.FILTERXML(_xlfn.WEBSERVICE("https://iss.moex.com/iss/engines/stock/markets/shares/securities/"&amp;B9&amp;"/candles.xml?from="&amp;$P$7&amp;"&amp;till="&amp;$P$7&amp;"&amp;interval=24"),"//document//data//rows//row/@low"),".",","))</f>
         <v>2.220000000000006</v>
       </c>
       <c r="R9" s="25">
@@ -1998,7 +2020,7 @@
         <v>1680</v>
       </c>
       <c r="H10" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="I10" s="24"/>
@@ -2015,15 +2037,15 @@
         <v>0.44000000000000483</v>
       </c>
       <c r="N10">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0.71000000000000085</v>
       </c>
       <c r="O10">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>1.230000000000004</v>
       </c>
       <c r="P10">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>1.3399999999999963</v>
       </c>
       <c r="R10" s="29">
@@ -2045,7 +2067,7 @@
         <v>50</v>
       </c>
       <c r="D11" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="E11" s="1">
@@ -2055,36 +2077,36 @@
         <v>0.2</v>
       </c>
       <c r="G11" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>403</v>
       </c>
       <c r="H11" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="I11" s="23"/>
       <c r="K11">
-        <f t="shared" ref="K11:K47" ca="1" si="6">ROUND(AVERAGE(L11:P11),2)</f>
+        <f t="shared" ref="K11:K47" ca="1" si="7">ROUND(AVERAGE(L11:P11),2)</f>
         <v>29.76</v>
       </c>
       <c r="L11">
-        <f t="shared" ref="L11:L47" ca="1" si="7">VALUE(SUBSTITUTE(_xlfn.FILTERXML(_xlfn.WEBSERVICE("https://iss.moex.com/iss/engines/stock/markets/shares/securities/"&amp;B11&amp;"/candles.xml?from="&amp;$L$7&amp;"&amp;till="&amp;$L$7&amp;"&amp;interval=24"),"//document//data//rows//row/@high"),".",","))-VALUE(SUBSTITUTE(_xlfn.FILTERXML(_xlfn.WEBSERVICE("https://iss.moex.com/iss/engines/stock/markets/shares/securities/"&amp;B11&amp;"/candles.xml?from="&amp;$L$7&amp;"&amp;till="&amp;$L$7&amp;"&amp;interval=24"),"//document//data//rows//row/@low"),".",","))</f>
+        <f t="shared" ref="L11:L47" ca="1" si="8">VALUE(SUBSTITUTE(_xlfn.FILTERXML(_xlfn.WEBSERVICE("https://iss.moex.com/iss/engines/stock/markets/shares/securities/"&amp;B11&amp;"/candles.xml?from="&amp;$L$7&amp;"&amp;till="&amp;$L$7&amp;"&amp;interval=24"),"//document//data//rows//row/@high"),".",","))-VALUE(SUBSTITUTE(_xlfn.FILTERXML(_xlfn.WEBSERVICE("https://iss.moex.com/iss/engines/stock/markets/shares/securities/"&amp;B11&amp;"/candles.xml?from="&amp;$L$7&amp;"&amp;till="&amp;$L$7&amp;"&amp;interval=24"),"//document//data//rows//row/@low"),".",","))</f>
         <v>17.200000000000045</v>
       </c>
       <c r="M11">
-        <f t="shared" ref="M11:M50" ca="1" si="8">VALUE(SUBSTITUTE(_xlfn.FILTERXML(_xlfn.WEBSERVICE("https://iss.moex.com/iss/engines/stock/markets/shares/securities/"&amp;B11&amp;"/candles.xml?from="&amp;$M$7&amp;"&amp;till="&amp;$M$7&amp;"&amp;interval=24"),"//document//data//rows//row/@high"),".",","))-VALUE(SUBSTITUTE(_xlfn.FILTERXML(_xlfn.WEBSERVICE("https://iss.moex.com/iss/engines/stock/markets/shares/securities/"&amp;B11&amp;"/candles.xml?from="&amp;$M$7&amp;"&amp;till="&amp;$M$7&amp;"&amp;interval=24"),"//document//data//rows//row/@low"),".",","))</f>
+        <f t="shared" ref="M11:M47" ca="1" si="9">VALUE(SUBSTITUTE(_xlfn.FILTERXML(_xlfn.WEBSERVICE("https://iss.moex.com/iss/engines/stock/markets/shares/securities/"&amp;B11&amp;"/candles.xml?from="&amp;$M$7&amp;"&amp;till="&amp;$M$7&amp;"&amp;interval=24"),"//document//data//rows//row/@high"),".",","))-VALUE(SUBSTITUTE(_xlfn.FILTERXML(_xlfn.WEBSERVICE("https://iss.moex.com/iss/engines/stock/markets/shares/securities/"&amp;B11&amp;"/candles.xml?from="&amp;$M$7&amp;"&amp;till="&amp;$M$7&amp;"&amp;interval=24"),"//document//data//rows//row/@low"),".",","))</f>
         <v>22</v>
       </c>
       <c r="N11">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="4"/>
         <v>20.799999999999955</v>
       </c>
       <c r="O11">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>33.800000000000068</v>
       </c>
       <c r="P11">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>55</v>
       </c>
       <c r="R11" s="29">
@@ -2106,7 +2128,7 @@
         <v>3.22</v>
       </c>
       <c r="D12" s="25">
-        <f t="shared" ref="D12:D17" si="9">C12/10</f>
+        <f t="shared" ref="D12:D17" si="10">C12/10</f>
         <v>0.32200000000000001</v>
       </c>
       <c r="E12" s="22">
@@ -2116,36 +2138,36 @@
         <v>0.1</v>
       </c>
       <c r="G12" s="26">
-        <f t="shared" ref="G12:G17" si="10">ROUND($C$4/(D12/E12*F12),0)</f>
+        <f t="shared" ref="G12:G17" si="11">ROUND($C$4/(D12/E12*F12),0)</f>
         <v>626</v>
       </c>
       <c r="H12" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="I12" s="24"/>
       <c r="K12">
+        <f t="shared" ca="1" si="7"/>
+        <v>1.7</v>
+      </c>
+      <c r="L12">
+        <f t="shared" ca="1" si="8"/>
+        <v>1.8599999999999994</v>
+      </c>
+      <c r="M12">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.71000000000000796</v>
+      </c>
+      <c r="N12">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.7800000000000011</v>
+      </c>
+      <c r="O12">
+        <f t="shared" ca="1" si="5"/>
+        <v>2.4100000000000108</v>
+      </c>
+      <c r="P12">
         <f t="shared" ca="1" si="6"/>
-        <v>1.7</v>
-      </c>
-      <c r="L12">
-        <f t="shared" ca="1" si="7"/>
-        <v>1.8599999999999994</v>
-      </c>
-      <c r="M12">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.71000000000000796</v>
-      </c>
-      <c r="N12">
-        <f t="shared" ca="1" si="3"/>
-        <v>1.7800000000000011</v>
-      </c>
-      <c r="O12">
-        <f t="shared" ca="1" si="4"/>
-        <v>2.4100000000000108</v>
-      </c>
-      <c r="P12">
-        <f t="shared" ca="1" si="5"/>
         <v>1.7199999999999989</v>
       </c>
       <c r="R12" s="29">
@@ -2165,7 +2187,7 @@
         <v>5.4</v>
       </c>
       <c r="D13" s="25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.54</v>
       </c>
       <c r="E13" s="22">
@@ -2175,36 +2197,36 @@
         <v>0.05</v>
       </c>
       <c r="G13" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3733</v>
       </c>
       <c r="H13" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="I13" s="23"/>
       <c r="K13">
+        <f t="shared" ca="1" si="7"/>
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="L13">
+        <f t="shared" ca="1" si="8"/>
+        <v>2.3499999999999943</v>
+      </c>
+      <c r="M13">
+        <f t="shared" ca="1" si="9"/>
+        <v>2.2999999999999829</v>
+      </c>
+      <c r="N13">
+        <f t="shared" ca="1" si="4"/>
+        <v>2.6500000000000057</v>
+      </c>
+      <c r="O13">
+        <f t="shared" ca="1" si="5"/>
+        <v>1.4500000000000171</v>
+      </c>
+      <c r="P13">
         <f t="shared" ca="1" si="6"/>
-        <v>2.2599999999999998</v>
-      </c>
-      <c r="L13">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.3499999999999943</v>
-      </c>
-      <c r="M13">
-        <f t="shared" ca="1" si="8"/>
-        <v>2.2999999999999829</v>
-      </c>
-      <c r="N13">
-        <f t="shared" ca="1" si="3"/>
-        <v>2.6500000000000057</v>
-      </c>
-      <c r="O13">
-        <f t="shared" ca="1" si="4"/>
-        <v>1.4500000000000171</v>
-      </c>
-      <c r="P13">
-        <f t="shared" ca="1" si="5"/>
         <v>2.5499999999999829</v>
       </c>
       <c r="R13" s="1"/>
@@ -2220,7 +2242,7 @@
         <v>1.8</v>
       </c>
       <c r="D14" s="25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.18</v>
       </c>
       <c r="E14" s="22">
@@ -2230,11 +2252,11 @@
         <v>0.1</v>
       </c>
       <c r="G14" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1120</v>
       </c>
       <c r="H14" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="I14" s="24"/>
@@ -2242,27 +2264,27 @@
         <v>46058</v>
       </c>
       <c r="K14">
+        <f t="shared" ca="1" si="7"/>
+        <v>2.4</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ca="1" si="8"/>
+        <v>2.1999999999999886</v>
+      </c>
+      <c r="M14">
+        <f t="shared" ca="1" si="9"/>
+        <v>1.5799999999999983</v>
+      </c>
+      <c r="N14">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.8800000000000097</v>
+      </c>
+      <c r="O14">
+        <f t="shared" ca="1" si="5"/>
+        <v>3.0800000000000125</v>
+      </c>
+      <c r="P14">
         <f t="shared" ca="1" si="6"/>
-        <v>2.4</v>
-      </c>
-      <c r="L14">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.1999999999999886</v>
-      </c>
-      <c r="M14">
-        <f t="shared" ca="1" si="8"/>
-        <v>1.5799999999999983</v>
-      </c>
-      <c r="N14">
-        <f t="shared" ca="1" si="3"/>
-        <v>1.8800000000000097</v>
-      </c>
-      <c r="O14">
-        <f t="shared" ca="1" si="4"/>
-        <v>3.0800000000000125</v>
-      </c>
-      <c r="P14">
-        <f t="shared" ca="1" si="5"/>
         <v>3.2599999999999909</v>
       </c>
       <c r="R14" s="25">
@@ -2284,7 +2306,7 @@
         <v>3.4</v>
       </c>
       <c r="D15" s="25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.33999999999999997</v>
       </c>
       <c r="E15" s="22">
@@ -2294,36 +2316,36 @@
         <v>0.2</v>
       </c>
       <c r="G15" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>593</v>
       </c>
       <c r="H15" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="I15" s="24"/>
       <c r="K15">
+        <f t="shared" ca="1" si="7"/>
+        <v>6.6</v>
+      </c>
+      <c r="L15">
+        <f t="shared" ca="1" si="8"/>
+        <v>7.2400000000000091</v>
+      </c>
+      <c r="M15">
+        <f t="shared" ca="1" si="9"/>
+        <v>2.8000000000000114</v>
+      </c>
+      <c r="N15">
+        <f t="shared" ca="1" si="4"/>
+        <v>6.3600000000000136</v>
+      </c>
+      <c r="O15">
+        <f t="shared" ca="1" si="5"/>
+        <v>10.099999999999994</v>
+      </c>
+      <c r="P15">
         <f t="shared" ca="1" si="6"/>
-        <v>6.6</v>
-      </c>
-      <c r="L15">
-        <f t="shared" ca="1" si="7"/>
-        <v>7.2400000000000091</v>
-      </c>
-      <c r="M15">
-        <f t="shared" ca="1" si="8"/>
-        <v>2.8000000000000114</v>
-      </c>
-      <c r="N15">
-        <f t="shared" ca="1" si="3"/>
-        <v>6.3600000000000136</v>
-      </c>
-      <c r="O15">
-        <f t="shared" ca="1" si="4"/>
-        <v>10.099999999999994</v>
-      </c>
-      <c r="P15">
-        <f t="shared" ca="1" si="5"/>
         <v>6.5199999999999818</v>
       </c>
       <c r="R15" s="25">
@@ -2343,7 +2365,7 @@
         <v>7.85E-2</v>
       </c>
       <c r="D16" s="25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7.8499999999999993E-3</v>
       </c>
       <c r="E16" s="22">
@@ -2353,36 +2375,36 @@
         <v>0.05</v>
       </c>
       <c r="G16" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2568</v>
       </c>
       <c r="H16" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="I16" s="24"/>
       <c r="K16">
+        <f t="shared" ca="1" si="7"/>
+        <v>-220617.61</v>
+      </c>
+      <c r="L16">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.11499999999999977</v>
+      </c>
+      <c r="M16">
+        <f t="shared" ca="1" si="9"/>
+        <v>-1131886</v>
+      </c>
+      <c r="N16">
+        <f t="shared" ca="1" si="4"/>
+        <v>1367469</v>
+      </c>
+      <c r="O16">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.15600000000000014</v>
+      </c>
+      <c r="P16">
         <f t="shared" ca="1" si="6"/>
-        <v>-220617.61</v>
-      </c>
-      <c r="L16">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.11499999999999977</v>
-      </c>
-      <c r="M16">
-        <f t="shared" ca="1" si="8"/>
-        <v>-1131886</v>
-      </c>
-      <c r="N16">
-        <f t="shared" ca="1" si="3"/>
-        <v>1367469</v>
-      </c>
-      <c r="O16">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.15600000000000014</v>
-      </c>
-      <c r="P16">
-        <f t="shared" ca="1" si="5"/>
         <v>-1338671.345</v>
       </c>
       <c r="R16" s="1"/>
@@ -2400,7 +2422,7 @@
         <v>110</v>
       </c>
       <c r="D17" s="25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11</v>
       </c>
       <c r="E17" s="22">
@@ -2410,37 +2432,37 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>183</v>
       </c>
       <c r="H17" s="22">
-        <f t="shared" ref="H17:H41" si="11">ROUND(D17/E17,0)</f>
+        <f t="shared" ref="H17:H41" si="12">ROUND(D17/E17,0)</f>
         <v>22</v>
       </c>
       <c r="I17" s="24"/>
       <c r="J17" s="30"/>
       <c r="K17">
+        <f t="shared" ca="1" si="7"/>
+        <v>108.4</v>
+      </c>
+      <c r="L17">
+        <f t="shared" ca="1" si="8"/>
+        <v>93.5</v>
+      </c>
+      <c r="M17">
+        <f t="shared" ca="1" si="9"/>
+        <v>68</v>
+      </c>
+      <c r="N17">
+        <f t="shared" ca="1" si="4"/>
+        <v>71</v>
+      </c>
+      <c r="O17">
+        <f t="shared" ca="1" si="5"/>
+        <v>114</v>
+      </c>
+      <c r="P17">
         <f t="shared" ca="1" si="6"/>
-        <v>108.4</v>
-      </c>
-      <c r="L17">
-        <f t="shared" ca="1" si="7"/>
-        <v>93.5</v>
-      </c>
-      <c r="M17">
-        <f t="shared" ca="1" si="8"/>
-        <v>68</v>
-      </c>
-      <c r="N17">
-        <f t="shared" ca="1" si="3"/>
-        <v>71</v>
-      </c>
-      <c r="O17">
-        <f t="shared" ca="1" si="4"/>
-        <v>114</v>
-      </c>
-      <c r="P17">
-        <f t="shared" ca="1" si="5"/>
         <v>195.5</v>
       </c>
       <c r="R17" s="25">
@@ -2462,7 +2484,7 @@
         <v>1.4</v>
       </c>
       <c r="D18" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.13999999999999999</v>
       </c>
       <c r="E18" s="1">
@@ -2472,36 +2494,36 @@
         <v>0.05</v>
       </c>
       <c r="G18" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1440</v>
       </c>
       <c r="H18" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>28</v>
       </c>
       <c r="I18" s="23"/>
       <c r="K18">
+        <f t="shared" ca="1" si="7"/>
+        <v>1.44</v>
+      </c>
+      <c r="L18">
+        <f t="shared" ca="1" si="8"/>
+        <v>1.1449999999999996</v>
+      </c>
+      <c r="M18">
+        <f t="shared" ca="1" si="9"/>
+        <v>1.4400000000000013</v>
+      </c>
+      <c r="N18">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.615000000000002</v>
+      </c>
+      <c r="O18">
+        <f t="shared" ca="1" si="5"/>
+        <v>1.1649999999999991</v>
+      </c>
+      <c r="P18">
         <f t="shared" ca="1" si="6"/>
-        <v>1.44</v>
-      </c>
-      <c r="L18">
-        <f t="shared" ca="1" si="7"/>
-        <v>1.1449999999999996</v>
-      </c>
-      <c r="M18">
-        <f t="shared" ca="1" si="8"/>
-        <v>1.4400000000000013</v>
-      </c>
-      <c r="N18">
-        <f t="shared" ca="1" si="3"/>
-        <v>1.615000000000002</v>
-      </c>
-      <c r="O18">
-        <f t="shared" ca="1" si="4"/>
-        <v>1.1649999999999991</v>
-      </c>
-      <c r="P18">
-        <f t="shared" ca="1" si="5"/>
         <v>1.8300000000000018</v>
       </c>
       <c r="R18" s="25">
@@ -2523,7 +2545,7 @@
         <v>150</v>
       </c>
       <c r="D19" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="E19" s="1">
@@ -2533,37 +2555,37 @@
         <v>0.5</v>
       </c>
       <c r="G19" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>134</v>
       </c>
       <c r="H19" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>30</v>
       </c>
       <c r="I19" s="23"/>
       <c r="J19" s="30"/>
       <c r="K19">
+        <f t="shared" ca="1" si="7"/>
+        <v>85.6</v>
+      </c>
+      <c r="L19">
+        <f t="shared" ca="1" si="8"/>
+        <v>89</v>
+      </c>
+      <c r="M19">
+        <f t="shared" ca="1" si="9"/>
+        <v>41</v>
+      </c>
+      <c r="N19">
+        <f t="shared" ca="1" si="4"/>
+        <v>88</v>
+      </c>
+      <c r="O19">
+        <f t="shared" ca="1" si="5"/>
+        <v>102</v>
+      </c>
+      <c r="P19">
         <f t="shared" ca="1" si="6"/>
-        <v>85.6</v>
-      </c>
-      <c r="L19">
-        <f t="shared" ca="1" si="7"/>
-        <v>89</v>
-      </c>
-      <c r="M19">
-        <f t="shared" ca="1" si="8"/>
-        <v>41</v>
-      </c>
-      <c r="N19">
-        <f t="shared" ca="1" si="3"/>
-        <v>88</v>
-      </c>
-      <c r="O19">
-        <f t="shared" ca="1" si="4"/>
-        <v>102</v>
-      </c>
-      <c r="P19">
-        <f t="shared" ca="1" si="5"/>
         <v>108</v>
       </c>
       <c r="R19" s="29">
@@ -2599,33 +2621,33 @@
         <v>354</v>
       </c>
       <c r="H20" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>57</v>
       </c>
       <c r="I20" s="24"/>
       <c r="J20" s="30"/>
       <c r="K20">
+        <f t="shared" ca="1" si="7"/>
+        <v>5.6</v>
+      </c>
+      <c r="L20">
+        <f t="shared" ca="1" si="8"/>
+        <v>7.0700000000000216</v>
+      </c>
+      <c r="M20">
+        <f t="shared" ca="1" si="9"/>
+        <v>8.1500000000000057</v>
+      </c>
+      <c r="N20">
+        <f t="shared" ca="1" si="4"/>
+        <v>3.3300000000000125</v>
+      </c>
+      <c r="O20">
+        <f t="shared" ca="1" si="5"/>
+        <v>5.0699999999999932</v>
+      </c>
+      <c r="P20">
         <f t="shared" ca="1" si="6"/>
-        <v>5.6</v>
-      </c>
-      <c r="L20">
-        <f t="shared" ca="1" si="7"/>
-        <v>7.0700000000000216</v>
-      </c>
-      <c r="M20">
-        <f t="shared" ca="1" si="8"/>
-        <v>8.1500000000000057</v>
-      </c>
-      <c r="N20">
-        <f t="shared" ca="1" si="3"/>
-        <v>3.3300000000000125</v>
-      </c>
-      <c r="O20">
-        <f t="shared" ca="1" si="4"/>
-        <v>5.0699999999999932</v>
-      </c>
-      <c r="P20">
-        <f t="shared" ca="1" si="5"/>
         <v>4.4000000000000057</v>
       </c>
       <c r="R20" s="25">
@@ -2647,7 +2669,7 @@
         <v>6.5</v>
       </c>
       <c r="D21" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.65</v>
       </c>
       <c r="E21" s="22">
@@ -2657,37 +2679,37 @@
         <v>0.01</v>
       </c>
       <c r="G21" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3102</v>
       </c>
       <c r="H21" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>65</v>
       </c>
       <c r="I21" s="23"/>
       <c r="J21" s="30"/>
       <c r="K21">
+        <f t="shared" ca="1" si="7"/>
+        <v>1.9</v>
+      </c>
+      <c r="L21">
+        <f t="shared" ca="1" si="8"/>
+        <v>1.8200000000000074</v>
+      </c>
+      <c r="M21">
+        <f t="shared" ca="1" si="9"/>
+        <v>1.2700000000000102</v>
+      </c>
+      <c r="N21">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.6300000000000097</v>
+      </c>
+      <c r="O21">
+        <f t="shared" ca="1" si="5"/>
+        <v>2.0699999999999932</v>
+      </c>
+      <c r="P21">
         <f t="shared" ca="1" si="6"/>
-        <v>1.9</v>
-      </c>
-      <c r="L21">
-        <f t="shared" ca="1" si="7"/>
-        <v>1.8200000000000074</v>
-      </c>
-      <c r="M21">
-        <f t="shared" ca="1" si="8"/>
-        <v>1.2700000000000102</v>
-      </c>
-      <c r="N21">
-        <f t="shared" ca="1" si="3"/>
-        <v>1.6300000000000097</v>
-      </c>
-      <c r="O21">
-        <f t="shared" ca="1" si="4"/>
-        <v>2.0699999999999932</v>
-      </c>
-      <c r="P21">
-        <f t="shared" ca="1" si="5"/>
         <v>2.7199999999999989</v>
       </c>
       <c r="R21" s="25">
@@ -2709,7 +2731,7 @@
         <v>6</v>
       </c>
       <c r="D22" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
       <c r="E22" s="1">
@@ -2719,36 +2741,36 @@
         <v>0.5</v>
       </c>
       <c r="G22" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>336</v>
       </c>
       <c r="H22" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>12</v>
       </c>
       <c r="I22" s="23"/>
       <c r="K22">
+        <f t="shared" ca="1" si="7"/>
+        <v>3.33</v>
+      </c>
+      <c r="L22">
+        <f t="shared" ca="1" si="8"/>
+        <v>3.5499999999999829</v>
+      </c>
+      <c r="M22">
+        <f t="shared" ca="1" si="9"/>
+        <v>3.5999999999999943</v>
+      </c>
+      <c r="N22">
+        <f t="shared" ca="1" si="4"/>
+        <v>4.2999999999999829</v>
+      </c>
+      <c r="O22">
+        <f t="shared" ca="1" si="5"/>
+        <v>2.0999999999999943</v>
+      </c>
+      <c r="P22">
         <f t="shared" ca="1" si="6"/>
-        <v>3.33</v>
-      </c>
-      <c r="L22">
-        <f t="shared" ca="1" si="7"/>
-        <v>3.5499999999999829</v>
-      </c>
-      <c r="M22">
-        <f t="shared" ca="1" si="8"/>
-        <v>3.5999999999999943</v>
-      </c>
-      <c r="N22">
-        <f t="shared" ca="1" si="3"/>
-        <v>4.2999999999999829</v>
-      </c>
-      <c r="O22">
-        <f t="shared" ca="1" si="4"/>
-        <v>2.0999999999999943</v>
-      </c>
-      <c r="P22">
-        <f t="shared" ca="1" si="5"/>
         <v>3.0999999999999943</v>
       </c>
       <c r="R22" s="25">
@@ -2770,7 +2792,7 @@
         <v>4</v>
       </c>
       <c r="D23" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
       <c r="E23" s="1">
@@ -2780,37 +2802,37 @@
         <v>0.2</v>
       </c>
       <c r="G23" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>504</v>
       </c>
       <c r="H23" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>20</v>
       </c>
       <c r="I23" s="23"/>
       <c r="J23" s="30"/>
       <c r="K23">
+        <f t="shared" ca="1" si="7"/>
+        <v>4.38</v>
+      </c>
+      <c r="L23">
+        <f t="shared" ca="1" si="8"/>
+        <v>3.980000000000004</v>
+      </c>
+      <c r="M23">
+        <f t="shared" ca="1" si="9"/>
+        <v>3.4399999999999977</v>
+      </c>
+      <c r="N23">
+        <f t="shared" ca="1" si="4"/>
+        <v>3.9200000000000017</v>
+      </c>
+      <c r="O23">
+        <f t="shared" ca="1" si="5"/>
+        <v>3.1600000000000108</v>
+      </c>
+      <c r="P23">
         <f t="shared" ca="1" si="6"/>
-        <v>4.38</v>
-      </c>
-      <c r="L23">
-        <f t="shared" ca="1" si="7"/>
-        <v>3.980000000000004</v>
-      </c>
-      <c r="M23">
-        <f t="shared" ca="1" si="8"/>
-        <v>3.4399999999999977</v>
-      </c>
-      <c r="N23">
-        <f t="shared" ca="1" si="3"/>
-        <v>3.9200000000000017</v>
-      </c>
-      <c r="O23">
-        <f t="shared" ca="1" si="4"/>
-        <v>3.1600000000000108</v>
-      </c>
-      <c r="P23">
-        <f t="shared" ca="1" si="5"/>
         <v>7.4000000000000057</v>
       </c>
       <c r="R23" s="29">
@@ -2846,32 +2868,32 @@
         <v>403</v>
       </c>
       <c r="H24" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>25</v>
       </c>
       <c r="I24" s="24"/>
       <c r="K24">
+        <f t="shared" ca="1" si="7"/>
+        <v>25.08</v>
+      </c>
+      <c r="L24">
+        <f t="shared" ca="1" si="8"/>
+        <v>25.5</v>
+      </c>
+      <c r="M24">
+        <f t="shared" ca="1" si="9"/>
+        <v>15.900000000000091</v>
+      </c>
+      <c r="N24">
+        <f t="shared" ca="1" si="4"/>
+        <v>12.799999999999955</v>
+      </c>
+      <c r="O24">
+        <f t="shared" ca="1" si="5"/>
+        <v>36.200000000000045</v>
+      </c>
+      <c r="P24">
         <f t="shared" ca="1" si="6"/>
-        <v>25.08</v>
-      </c>
-      <c r="L24">
-        <f t="shared" ca="1" si="7"/>
-        <v>25.5</v>
-      </c>
-      <c r="M24">
-        <f t="shared" ca="1" si="8"/>
-        <v>15.900000000000091</v>
-      </c>
-      <c r="N24">
-        <f t="shared" ca="1" si="3"/>
-        <v>12.799999999999955</v>
-      </c>
-      <c r="O24">
-        <f t="shared" ca="1" si="4"/>
-        <v>36.200000000000045</v>
-      </c>
-      <c r="P24">
-        <f t="shared" ca="1" si="5"/>
         <v>35</v>
       </c>
       <c r="R24" s="1"/>
@@ -2889,7 +2911,7 @@
         <v>100</v>
       </c>
       <c r="D25" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="E25" s="1">
@@ -2899,37 +2921,37 @@
         <v>0.5</v>
       </c>
       <c r="G25" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>202</v>
       </c>
       <c r="H25" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>20</v>
       </c>
       <c r="I25" s="23"/>
       <c r="J25" s="30"/>
       <c r="K25">
+        <f t="shared" ca="1" si="7"/>
+        <v>125.5</v>
+      </c>
+      <c r="L25">
+        <f t="shared" ca="1" si="8"/>
+        <v>88.5</v>
+      </c>
+      <c r="M25">
+        <f t="shared" ca="1" si="9"/>
+        <v>110.5</v>
+      </c>
+      <c r="N25">
+        <f t="shared" ca="1" si="4"/>
+        <v>152</v>
+      </c>
+      <c r="O25">
+        <f t="shared" ca="1" si="5"/>
+        <v>208.5</v>
+      </c>
+      <c r="P25">
         <f t="shared" ca="1" si="6"/>
-        <v>125.5</v>
-      </c>
-      <c r="L25">
-        <f t="shared" ca="1" si="7"/>
-        <v>88.5</v>
-      </c>
-      <c r="M25">
-        <f t="shared" ca="1" si="8"/>
-        <v>110.5</v>
-      </c>
-      <c r="N25">
-        <f t="shared" ca="1" si="3"/>
-        <v>152</v>
-      </c>
-      <c r="O25">
-        <f t="shared" ca="1" si="4"/>
-        <v>208.5</v>
-      </c>
-      <c r="P25">
-        <f t="shared" ca="1" si="5"/>
         <v>68</v>
       </c>
       <c r="R25" s="25">
@@ -2965,32 +2987,32 @@
         <v>144</v>
       </c>
       <c r="H26" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>70</v>
       </c>
       <c r="I26" s="24"/>
       <c r="K26">
+        <f t="shared" ca="1" si="7"/>
+        <v>44.04</v>
+      </c>
+      <c r="L26">
+        <f t="shared" ca="1" si="8"/>
+        <v>55.799999999999955</v>
+      </c>
+      <c r="M26">
+        <f t="shared" ca="1" si="9"/>
+        <v>23.599999999999909</v>
+      </c>
+      <c r="N26">
+        <f t="shared" ca="1" si="4"/>
+        <v>53</v>
+      </c>
+      <c r="O26">
+        <f t="shared" ca="1" si="5"/>
+        <v>35.399999999999864</v>
+      </c>
+      <c r="P26">
         <f t="shared" ca="1" si="6"/>
-        <v>44.04</v>
-      </c>
-      <c r="L26">
-        <f t="shared" ca="1" si="7"/>
-        <v>55.799999999999955</v>
-      </c>
-      <c r="M26">
-        <f t="shared" ca="1" si="8"/>
-        <v>23.599999999999909</v>
-      </c>
-      <c r="N26">
-        <f t="shared" ca="1" si="3"/>
-        <v>53</v>
-      </c>
-      <c r="O26">
-        <f t="shared" ca="1" si="4"/>
-        <v>35.399999999999864</v>
-      </c>
-      <c r="P26">
-        <f t="shared" ca="1" si="5"/>
         <v>52.400000000000091</v>
       </c>
       <c r="R26" s="1"/>
@@ -3008,7 +3030,7 @@
         <v>112</v>
       </c>
       <c r="D27" s="25">
-        <f t="shared" ref="D27:D40" si="12">C27/10</f>
+        <f t="shared" ref="D27:D40" si="13">C27/10</f>
         <v>11.2</v>
       </c>
       <c r="E27" s="22">
@@ -3018,36 +3040,36 @@
         <v>1</v>
       </c>
       <c r="G27" s="26">
-        <f t="shared" ref="G27:G40" si="13">ROUND($C$4/(D27/E27*F27),0)</f>
+        <f t="shared" ref="G27:G40" si="14">ROUND($C$4/(D27/E27*F27),0)</f>
         <v>180</v>
       </c>
       <c r="H27" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11</v>
       </c>
       <c r="I27" s="24"/>
       <c r="K27">
+        <f t="shared" ca="1" si="7"/>
+        <v>95</v>
+      </c>
+      <c r="L27">
+        <f t="shared" ca="1" si="8"/>
+        <v>83</v>
+      </c>
+      <c r="M27">
+        <f t="shared" ca="1" si="9"/>
+        <v>67</v>
+      </c>
+      <c r="N27">
+        <f t="shared" ca="1" si="4"/>
+        <v>108</v>
+      </c>
+      <c r="O27">
+        <f t="shared" ca="1" si="5"/>
+        <v>125</v>
+      </c>
+      <c r="P27">
         <f t="shared" ca="1" si="6"/>
-        <v>95</v>
-      </c>
-      <c r="L27">
-        <f t="shared" ca="1" si="7"/>
-        <v>83</v>
-      </c>
-      <c r="M27">
-        <f t="shared" ca="1" si="8"/>
-        <v>67</v>
-      </c>
-      <c r="N27">
-        <f t="shared" ca="1" si="3"/>
-        <v>108</v>
-      </c>
-      <c r="O27">
-        <f t="shared" ca="1" si="4"/>
-        <v>125</v>
-      </c>
-      <c r="P27">
-        <f t="shared" ca="1" si="5"/>
         <v>92</v>
       </c>
       <c r="R27" s="25">
@@ -3081,32 +3103,32 @@
         <v>604</v>
       </c>
       <c r="H28" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>33</v>
       </c>
       <c r="I28" s="24"/>
       <c r="K28">
+        <f t="shared" ca="1" si="7"/>
+        <v>14.14</v>
+      </c>
+      <c r="L28">
+        <f t="shared" ca="1" si="8"/>
+        <v>32.100000000000023</v>
+      </c>
+      <c r="M28">
+        <f t="shared" ca="1" si="9"/>
+        <v>7.8999999999999773</v>
+      </c>
+      <c r="N28">
+        <f t="shared" ca="1" si="4"/>
+        <v>6.3000000000000114</v>
+      </c>
+      <c r="O28">
+        <f t="shared" ca="1" si="5"/>
+        <v>12.399999999999977</v>
+      </c>
+      <c r="P28">
         <f t="shared" ca="1" si="6"/>
-        <v>14.14</v>
-      </c>
-      <c r="L28">
-        <f t="shared" ca="1" si="7"/>
-        <v>32.100000000000023</v>
-      </c>
-      <c r="M28">
-        <f t="shared" ca="1" si="8"/>
-        <v>7.8999999999999773</v>
-      </c>
-      <c r="N28">
-        <f t="shared" ca="1" si="3"/>
-        <v>6.3000000000000114</v>
-      </c>
-      <c r="O28">
-        <f t="shared" ca="1" si="4"/>
-        <v>12.399999999999977</v>
-      </c>
-      <c r="P28">
-        <f t="shared" ca="1" si="5"/>
         <v>12</v>
       </c>
       <c r="R28" s="1"/>
@@ -3126,7 +3148,7 @@
         <v>520</v>
       </c>
       <c r="D29" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>52</v>
       </c>
       <c r="E29" s="22">
@@ -3136,37 +3158,37 @@
         <v>0.5</v>
       </c>
       <c r="G29" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>39</v>
       </c>
       <c r="H29" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>104</v>
       </c>
       <c r="I29" s="24"/>
       <c r="J29" s="30"/>
       <c r="K29">
+        <f t="shared" ca="1" si="7"/>
+        <v>109.84</v>
+      </c>
+      <c r="L29">
+        <f t="shared" ca="1" si="8"/>
+        <v>81</v>
+      </c>
+      <c r="M29">
+        <f t="shared" ca="1" si="9"/>
+        <v>48</v>
+      </c>
+      <c r="N29">
+        <f t="shared" ca="1" si="4"/>
+        <v>132.20000000000027</v>
+      </c>
+      <c r="O29">
+        <f t="shared" ca="1" si="5"/>
+        <v>143</v>
+      </c>
+      <c r="P29">
         <f t="shared" ca="1" si="6"/>
-        <v>109.84</v>
-      </c>
-      <c r="L29">
-        <f t="shared" ca="1" si="7"/>
-        <v>81</v>
-      </c>
-      <c r="M29">
-        <f t="shared" ca="1" si="8"/>
-        <v>48</v>
-      </c>
-      <c r="N29">
-        <f t="shared" ca="1" si="3"/>
-        <v>132.20000000000027</v>
-      </c>
-      <c r="O29">
-        <f t="shared" ca="1" si="4"/>
-        <v>143</v>
-      </c>
-      <c r="P29">
-        <f t="shared" ca="1" si="5"/>
         <v>145</v>
       </c>
       <c r="R29" s="25">
@@ -3186,7 +3208,7 @@
         <v>10</v>
       </c>
       <c r="D30" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="E30" s="22">
@@ -3196,36 +3218,36 @@
         <v>0.05</v>
       </c>
       <c r="G30" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2016</v>
       </c>
       <c r="H30" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>20</v>
       </c>
       <c r="I30" s="24"/>
       <c r="K30">
+        <f t="shared" ca="1" si="7"/>
+        <v>5.08</v>
+      </c>
+      <c r="L30">
+        <f t="shared" ca="1" si="8"/>
+        <v>3.3000000000000114</v>
+      </c>
+      <c r="M30">
+        <f t="shared" ca="1" si="9"/>
+        <v>3.1999999999999886</v>
+      </c>
+      <c r="N30">
+        <f t="shared" ca="1" si="4"/>
+        <v>3.1000000000000085</v>
+      </c>
+      <c r="O30">
+        <f t="shared" ca="1" si="5"/>
+        <v>4.7999999999999972</v>
+      </c>
+      <c r="P30">
         <f t="shared" ca="1" si="6"/>
-        <v>5.08</v>
-      </c>
-      <c r="L30">
-        <f t="shared" ca="1" si="7"/>
-        <v>3.3000000000000114</v>
-      </c>
-      <c r="M30">
-        <f t="shared" ca="1" si="8"/>
-        <v>3.1999999999999886</v>
-      </c>
-      <c r="N30">
-        <f t="shared" ca="1" si="3"/>
-        <v>3.1000000000000085</v>
-      </c>
-      <c r="O30">
-        <f t="shared" ca="1" si="4"/>
-        <v>4.7999999999999972</v>
-      </c>
-      <c r="P30">
-        <f t="shared" ca="1" si="5"/>
         <v>11</v>
       </c>
       <c r="R30" s="1"/>
@@ -3243,7 +3265,7 @@
         <v>7.51</v>
       </c>
       <c r="D31" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.751</v>
       </c>
       <c r="E31" s="22">
@@ -3253,11 +3275,11 @@
         <v>0.05</v>
       </c>
       <c r="G31" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2684</v>
       </c>
       <c r="H31" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>15</v>
       </c>
       <c r="I31" s="23"/>
@@ -3265,27 +3287,27 @@
         <v>46058</v>
       </c>
       <c r="K31">
+        <f t="shared" ca="1" si="7"/>
+        <v>7.51</v>
+      </c>
+      <c r="L31">
+        <f t="shared" ca="1" si="8"/>
+        <v>5.9499999999999886</v>
+      </c>
+      <c r="M31">
+        <f t="shared" ca="1" si="9"/>
+        <v>4.75</v>
+      </c>
+      <c r="N31">
+        <f t="shared" ca="1" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="O31">
+        <f t="shared" ca="1" si="5"/>
+        <v>7.8999999999999773</v>
+      </c>
+      <c r="P31">
         <f t="shared" ca="1" si="6"/>
-        <v>7.51</v>
-      </c>
-      <c r="L31">
-        <f t="shared" ca="1" si="7"/>
-        <v>5.9499999999999886</v>
-      </c>
-      <c r="M31">
-        <f t="shared" ca="1" si="8"/>
-        <v>4.75</v>
-      </c>
-      <c r="N31">
-        <f t="shared" ca="1" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="O31">
-        <f t="shared" ca="1" si="4"/>
-        <v>7.8999999999999773</v>
-      </c>
-      <c r="P31">
-        <f t="shared" ca="1" si="5"/>
         <v>9.9499999999999886</v>
       </c>
       <c r="R31" s="29">
@@ -3321,32 +3343,32 @@
         <v>1792</v>
       </c>
       <c r="H32" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>23</v>
       </c>
       <c r="I32" s="24"/>
       <c r="K32">
+        <f t="shared" ca="1" si="7"/>
+        <v>1.99</v>
+      </c>
+      <c r="L32">
+        <f t="shared" ca="1" si="8"/>
+        <v>1.75</v>
+      </c>
+      <c r="M32">
+        <f t="shared" ca="1" si="9"/>
+        <v>1.0900000000000034</v>
+      </c>
+      <c r="N32">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.2650000000000006</v>
+      </c>
+      <c r="O32">
+        <f t="shared" ca="1" si="5"/>
+        <v>2.5849999999999937</v>
+      </c>
+      <c r="P32">
         <f t="shared" ca="1" si="6"/>
-        <v>1.99</v>
-      </c>
-      <c r="L32">
-        <f t="shared" ca="1" si="7"/>
-        <v>1.75</v>
-      </c>
-      <c r="M32">
-        <f t="shared" ca="1" si="8"/>
-        <v>1.0900000000000034</v>
-      </c>
-      <c r="N32">
-        <f t="shared" ca="1" si="3"/>
-        <v>1.2650000000000006</v>
-      </c>
-      <c r="O32">
-        <f t="shared" ca="1" si="4"/>
-        <v>2.5849999999999937</v>
-      </c>
-      <c r="P32">
-        <f t="shared" ca="1" si="5"/>
         <v>3.25</v>
       </c>
       <c r="R32" s="1"/>
@@ -3364,7 +3386,7 @@
         <v>6</v>
       </c>
       <c r="D33" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.6</v>
       </c>
       <c r="E33" s="22">
@@ -3374,37 +3396,37 @@
         <v>0.1</v>
       </c>
       <c r="G33" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>336</v>
       </c>
       <c r="H33" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>60</v>
       </c>
       <c r="I33" s="23"/>
       <c r="J33" s="30"/>
       <c r="K33">
+        <f t="shared" ca="1" si="7"/>
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="L33">
+        <f t="shared" ca="1" si="8"/>
+        <v>2.6299999999999955</v>
+      </c>
+      <c r="M33">
+        <f t="shared" ca="1" si="9"/>
+        <v>2.1700000000000159</v>
+      </c>
+      <c r="N33">
+        <f t="shared" ca="1" si="4"/>
+        <v>4.4900000000000091</v>
+      </c>
+      <c r="O33">
+        <f t="shared" ca="1" si="5"/>
+        <v>4.5799999999999841</v>
+      </c>
+      <c r="P33">
         <f t="shared" ca="1" si="6"/>
-        <v>4.3600000000000003</v>
-      </c>
-      <c r="L33">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.6299999999999955</v>
-      </c>
-      <c r="M33">
-        <f t="shared" ca="1" si="8"/>
-        <v>2.1700000000000159</v>
-      </c>
-      <c r="N33">
-        <f t="shared" ca="1" si="3"/>
-        <v>4.4900000000000091</v>
-      </c>
-      <c r="O33">
-        <f t="shared" ca="1" si="4"/>
-        <v>4.5799999999999841</v>
-      </c>
-      <c r="P33">
-        <f t="shared" ca="1" si="5"/>
         <v>7.910000000000025</v>
       </c>
       <c r="R33" s="29">
@@ -3426,7 +3448,7 @@
         <v>70</v>
       </c>
       <c r="D34" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7</v>
       </c>
       <c r="E34" s="22">
@@ -3436,36 +3458,36 @@
         <v>0.2</v>
       </c>
       <c r="G34" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>288</v>
       </c>
       <c r="H34" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>35</v>
       </c>
       <c r="I34" s="24"/>
       <c r="K34">
+        <f t="shared" ca="1" si="7"/>
+        <v>44.16</v>
+      </c>
+      <c r="L34">
+        <f t="shared" ca="1" si="8"/>
+        <v>41</v>
+      </c>
+      <c r="M34">
+        <f t="shared" ca="1" si="9"/>
+        <v>43</v>
+      </c>
+      <c r="N34">
+        <f t="shared" ca="1" si="4"/>
+        <v>55.200000000000045</v>
+      </c>
+      <c r="O34">
+        <f t="shared" ca="1" si="5"/>
+        <v>52.200000000000045</v>
+      </c>
+      <c r="P34">
         <f t="shared" ca="1" si="6"/>
-        <v>44.16</v>
-      </c>
-      <c r="L34">
-        <f t="shared" ca="1" si="7"/>
-        <v>41</v>
-      </c>
-      <c r="M34">
-        <f t="shared" ca="1" si="8"/>
-        <v>43</v>
-      </c>
-      <c r="N34">
-        <f t="shared" ca="1" si="3"/>
-        <v>55.200000000000045</v>
-      </c>
-      <c r="O34">
-        <f t="shared" ca="1" si="4"/>
-        <v>52.200000000000045</v>
-      </c>
-      <c r="P34">
-        <f t="shared" ca="1" si="5"/>
         <v>29.399999999999977</v>
       </c>
       <c r="R34" s="25">
@@ -3499,32 +3521,32 @@
         <v>1440</v>
       </c>
       <c r="H35" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>14</v>
       </c>
       <c r="I35" s="24"/>
       <c r="K35">
+        <f t="shared" ca="1" si="7"/>
+        <v>-34552.17</v>
+      </c>
+      <c r="L35">
+        <f t="shared" ca="1" si="8"/>
+        <v>5.1999999999999824E-2</v>
+      </c>
+      <c r="M35">
+        <f t="shared" ca="1" si="9"/>
+        <v>-184448.73800000001</v>
+      </c>
+      <c r="N35">
+        <f t="shared" ca="1" si="4"/>
+        <v>3.499999999999992E-2</v>
+      </c>
+      <c r="O35">
+        <f t="shared" ca="1" si="5"/>
+        <v>4.8999999999999932E-2</v>
+      </c>
+      <c r="P35">
         <f t="shared" ca="1" si="6"/>
-        <v>-34552.17</v>
-      </c>
-      <c r="L35">
-        <f t="shared" ca="1" si="7"/>
-        <v>5.1999999999999824E-2</v>
-      </c>
-      <c r="M35">
-        <f t="shared" ca="1" si="8"/>
-        <v>-184448.73800000001</v>
-      </c>
-      <c r="N35">
-        <f t="shared" ca="1" si="3"/>
-        <v>3.499999999999992E-2</v>
-      </c>
-      <c r="O35">
-        <f t="shared" ca="1" si="4"/>
-        <v>4.8999999999999932E-2</v>
-      </c>
-      <c r="P35">
-        <f t="shared" ca="1" si="5"/>
         <v>11687.748</v>
       </c>
       <c r="R35" s="29">
@@ -3556,32 +3578,32 @@
         <v>1084</v>
       </c>
       <c r="H36" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>37</v>
       </c>
       <c r="I36" s="24"/>
       <c r="K36">
+        <f t="shared" ca="1" si="7"/>
+        <v>9.75</v>
+      </c>
+      <c r="L36">
+        <f t="shared" ca="1" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="M36">
+        <f t="shared" ca="1" si="9"/>
+        <v>5.8000000000000114</v>
+      </c>
+      <c r="N36">
+        <f t="shared" ca="1" si="4"/>
+        <v>9.4000000000000341</v>
+      </c>
+      <c r="O36">
+        <f t="shared" ca="1" si="5"/>
+        <v>11.25</v>
+      </c>
+      <c r="P36">
         <f t="shared" ca="1" si="6"/>
-        <v>9.75</v>
-      </c>
-      <c r="L36">
-        <f t="shared" ca="1" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="M36">
-        <f t="shared" ca="1" si="8"/>
-        <v>5.8000000000000114</v>
-      </c>
-      <c r="N36">
-        <f t="shared" ca="1" si="3"/>
-        <v>9.4000000000000341</v>
-      </c>
-      <c r="O36">
-        <f t="shared" ca="1" si="4"/>
-        <v>11.25</v>
-      </c>
-      <c r="P36">
-        <f t="shared" ca="1" si="5"/>
         <v>14.300000000000011</v>
       </c>
       <c r="R36" s="25">
@@ -3615,7 +3637,7 @@
         <v>336</v>
       </c>
       <c r="H37" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>30</v>
       </c>
       <c r="I37" s="24"/>
@@ -3623,27 +3645,27 @@
         <v>46058</v>
       </c>
       <c r="K37">
+        <f t="shared" ca="1" si="7"/>
+        <v>45.6</v>
+      </c>
+      <c r="L37">
+        <f t="shared" ca="1" si="8"/>
+        <v>115</v>
+      </c>
+      <c r="M37">
+        <f t="shared" ca="1" si="9"/>
+        <v>22</v>
+      </c>
+      <c r="N37">
+        <f t="shared" ca="1" si="4"/>
+        <v>15.5</v>
+      </c>
+      <c r="O37">
+        <f t="shared" ca="1" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="P37">
         <f t="shared" ca="1" si="6"/>
-        <v>45.6</v>
-      </c>
-      <c r="L37">
-        <f t="shared" ca="1" si="7"/>
-        <v>115</v>
-      </c>
-      <c r="M37">
-        <f t="shared" ca="1" si="8"/>
-        <v>22</v>
-      </c>
-      <c r="N37">
-        <f t="shared" ca="1" si="3"/>
-        <v>15.5</v>
-      </c>
-      <c r="O37">
-        <f t="shared" ca="1" si="4"/>
-        <v>40</v>
-      </c>
-      <c r="P37">
-        <f t="shared" ca="1" si="5"/>
         <v>35.5</v>
       </c>
       <c r="R37" s="1"/>
@@ -3675,32 +3697,32 @@
         <v>0</v>
       </c>
       <c r="H38" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>13800</v>
       </c>
       <c r="I38" s="24"/>
       <c r="K38">
+        <f t="shared" ca="1" si="7"/>
+        <v>-18487.09</v>
+      </c>
+      <c r="L38">
+        <f t="shared" ca="1" si="8"/>
+        <v>-46264.525000000001</v>
+      </c>
+      <c r="M38">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.26500000000000057</v>
+      </c>
+      <c r="N38">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.54499999999999815</v>
+      </c>
+      <c r="O38">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.49500000000000099</v>
+      </c>
+      <c r="P38">
         <f t="shared" ca="1" si="6"/>
-        <v>-18487.09</v>
-      </c>
-      <c r="L38">
-        <f t="shared" ca="1" si="7"/>
-        <v>-46264.525000000001</v>
-      </c>
-      <c r="M38">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.26500000000000057</v>
-      </c>
-      <c r="N38">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.54499999999999815</v>
-      </c>
-      <c r="O38">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.49500000000000099</v>
-      </c>
-      <c r="P38">
-        <f t="shared" ca="1" si="5"/>
         <v>-46172.25</v>
       </c>
     </row>
@@ -3712,7 +3734,7 @@
         <v>1.65</v>
       </c>
       <c r="D39" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.16499999999999998</v>
       </c>
       <c r="E39" s="22">
@@ -3722,36 +3744,36 @@
         <v>0.05</v>
       </c>
       <c r="G39" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1222</v>
       </c>
       <c r="H39" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>33</v>
       </c>
       <c r="I39" s="24"/>
       <c r="K39">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.79</v>
+      </c>
+      <c r="L39">
+        <f t="shared" ca="1" si="8"/>
+        <v>1.0300000000000011</v>
+      </c>
+      <c r="M39">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.42999999999999972</v>
+      </c>
+      <c r="N39">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.86999999999999744</v>
+      </c>
+      <c r="O39">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.57999999999999829</v>
+      </c>
+      <c r="P39">
         <f t="shared" ca="1" si="6"/>
-        <v>0.79</v>
-      </c>
-      <c r="L39">
-        <f t="shared" ca="1" si="7"/>
-        <v>1.0300000000000011</v>
-      </c>
-      <c r="M39">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.42999999999999972</v>
-      </c>
-      <c r="N39">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.86999999999999744</v>
-      </c>
-      <c r="O39">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.57999999999999829</v>
-      </c>
-      <c r="P39">
-        <f t="shared" ca="1" si="5"/>
         <v>1.0649999999999977</v>
       </c>
       <c r="R39" s="25">
@@ -3773,7 +3795,7 @@
         <v>12</v>
       </c>
       <c r="D40" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.2</v>
       </c>
       <c r="E40" s="22">
@@ -3783,16 +3805,16 @@
         <v>0.1</v>
       </c>
       <c r="G40" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1680</v>
       </c>
       <c r="H40" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>12</v>
       </c>
       <c r="I40" s="24"/>
       <c r="K40">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="7"/>
         <v>13.62</v>
       </c>
       <c r="L40">
@@ -3800,19 +3822,19 @@
         <v>14.899999999999977</v>
       </c>
       <c r="M40">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>8.8000000000000682</v>
       </c>
       <c r="N40">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="4"/>
         <v>13.700000000000045</v>
       </c>
       <c r="O40">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>12.199999999999932</v>
       </c>
       <c r="P40">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>18.5</v>
       </c>
       <c r="R40" s="25">
@@ -3842,36 +3864,36 @@
         <v>0.2</v>
       </c>
       <c r="G41" s="26">
-        <f t="shared" ref="G41:G46" si="14">ROUND($C$4/(D41/E41*F41),0)</f>
+        <f t="shared" ref="G41:G46" si="15">ROUND($C$4/(D41/E41*F41),0)</f>
         <v>336</v>
       </c>
       <c r="H41" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>30</v>
       </c>
       <c r="I41" s="24"/>
       <c r="K41">
+        <f t="shared" ca="1" si="7"/>
+        <v>2.63</v>
+      </c>
+      <c r="L41">
+        <f t="shared" ca="1" si="8"/>
+        <v>3.3599999999999994</v>
+      </c>
+      <c r="M41">
+        <f t="shared" ca="1" si="9"/>
+        <v>2.1999999999999886</v>
+      </c>
+      <c r="N41">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.6599999999999966</v>
+      </c>
+      <c r="O41">
+        <f t="shared" ca="1" si="5"/>
+        <v>2.0600000000000023</v>
+      </c>
+      <c r="P41">
         <f t="shared" ca="1" si="6"/>
-        <v>2.63</v>
-      </c>
-      <c r="L41">
-        <f t="shared" ca="1" si="7"/>
-        <v>3.3599999999999994</v>
-      </c>
-      <c r="M41">
-        <f t="shared" ca="1" si="8"/>
-        <v>2.1999999999999886</v>
-      </c>
-      <c r="N41">
-        <f t="shared" ca="1" si="3"/>
-        <v>1.6599999999999966</v>
-      </c>
-      <c r="O41">
-        <f t="shared" ca="1" si="4"/>
-        <v>2.0600000000000023</v>
-      </c>
-      <c r="P41">
-        <f t="shared" ca="1" si="5"/>
         <v>3.8799999999999955</v>
       </c>
       <c r="R41" s="29">
@@ -3901,36 +3923,36 @@
         <v>0.5</v>
       </c>
       <c r="G42" s="26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>288</v>
       </c>
       <c r="H42" s="22">
-        <f t="shared" ref="H42:H44" si="15">ROUND(D42/E42,0)</f>
+        <f t="shared" ref="H42:H44" si="16">ROUND(D42/E42,0)</f>
         <v>14</v>
       </c>
       <c r="I42" s="24"/>
       <c r="K42">
+        <f t="shared" ca="1" si="7"/>
+        <v>17.04</v>
+      </c>
+      <c r="L42">
+        <f t="shared" ca="1" si="8"/>
+        <v>18.399999999999864</v>
+      </c>
+      <c r="M42">
+        <f t="shared" ca="1" si="9"/>
+        <v>9.8000000000001819</v>
+      </c>
+      <c r="N42">
+        <f t="shared" ca="1" si="4"/>
+        <v>22.799999999999955</v>
+      </c>
+      <c r="O42">
+        <f t="shared" ca="1" si="5"/>
+        <v>15.599999999999909</v>
+      </c>
+      <c r="P42">
         <f t="shared" ca="1" si="6"/>
-        <v>17.04</v>
-      </c>
-      <c r="L42">
-        <f t="shared" ca="1" si="7"/>
-        <v>18.399999999999864</v>
-      </c>
-      <c r="M42">
-        <f t="shared" ca="1" si="8"/>
-        <v>9.8000000000001819</v>
-      </c>
-      <c r="N42">
-        <f t="shared" ca="1" si="3"/>
-        <v>22.799999999999955</v>
-      </c>
-      <c r="O42">
-        <f t="shared" ca="1" si="4"/>
-        <v>15.599999999999909</v>
-      </c>
-      <c r="P42">
-        <f t="shared" ca="1" si="5"/>
         <v>18.599999999999909</v>
       </c>
       <c r="R42" s="1"/>
@@ -3960,11 +3982,11 @@
         <v>0.1</v>
       </c>
       <c r="G43" s="26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>395</v>
       </c>
       <c r="H43" s="22">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>51</v>
       </c>
       <c r="I43" s="24"/>
@@ -3976,23 +3998,23 @@
         <v>0.12180000000000001</v>
       </c>
       <c r="L43">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>8.2900000000000085E-2</v>
       </c>
       <c r="M43">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>7.6999999999999957E-2</v>
       </c>
       <c r="N43">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="4"/>
         <v>5.2799999999999958E-2</v>
       </c>
       <c r="O43">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>8.890000000000009E-2</v>
       </c>
       <c r="P43">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0.3073999999999999</v>
       </c>
       <c r="R43" s="1"/>
@@ -4018,11 +4040,11 @@
         <v>0.05</v>
       </c>
       <c r="G44" s="26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2076</v>
       </c>
       <c r="H44" s="22">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>19</v>
       </c>
       <c r="I44" s="23"/>
@@ -4030,27 +4052,27 @@
         <v>46058</v>
       </c>
       <c r="K44">
+        <f t="shared" ca="1" si="7"/>
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="L44">
+        <f t="shared" ca="1" si="8"/>
+        <v>10.449999999999989</v>
+      </c>
+      <c r="M44">
+        <f t="shared" ca="1" si="9"/>
+        <v>12.600000000000023</v>
+      </c>
+      <c r="N44">
+        <f t="shared" ca="1" si="4"/>
+        <v>7.5999999999999659</v>
+      </c>
+      <c r="O44">
+        <f t="shared" ca="1" si="5"/>
+        <v>7.6999999999999886</v>
+      </c>
+      <c r="P44">
         <f t="shared" ca="1" si="6"/>
-        <v>9.7100000000000009</v>
-      </c>
-      <c r="L44">
-        <f t="shared" ca="1" si="7"/>
-        <v>10.449999999999989</v>
-      </c>
-      <c r="M44">
-        <f t="shared" ca="1" si="8"/>
-        <v>12.600000000000023</v>
-      </c>
-      <c r="N44">
-        <f t="shared" ca="1" si="3"/>
-        <v>7.5999999999999659</v>
-      </c>
-      <c r="O44">
-        <f t="shared" ca="1" si="4"/>
-        <v>7.6999999999999886</v>
-      </c>
-      <c r="P44">
-        <f t="shared" ca="1" si="5"/>
         <v>10.200000000000045</v>
       </c>
       <c r="R44" s="1"/>
@@ -4081,7 +4103,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G45" s="26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>7724</v>
       </c>
       <c r="H45" s="22">
@@ -4093,27 +4115,27 @@
         <v>46057</v>
       </c>
       <c r="K45">
+        <f t="shared" ca="1" si="7"/>
+        <v>3.58</v>
+      </c>
+      <c r="L45">
+        <f t="shared" ca="1" si="8"/>
+        <v>2.4749999999999943</v>
+      </c>
+      <c r="M45">
+        <f t="shared" ca="1" si="9"/>
+        <v>2.6299999999999955</v>
+      </c>
+      <c r="N45">
+        <f t="shared" ca="1" si="4"/>
+        <v>4.5100000000000051</v>
+      </c>
+      <c r="O45">
+        <f t="shared" ca="1" si="5"/>
+        <v>3.4400000000000119</v>
+      </c>
+      <c r="P45">
         <f t="shared" ca="1" si="6"/>
-        <v>3.58</v>
-      </c>
-      <c r="L45">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.4749999999999943</v>
-      </c>
-      <c r="M45">
-        <f t="shared" ca="1" si="8"/>
-        <v>2.6299999999999955</v>
-      </c>
-      <c r="N45">
-        <f t="shared" ca="1" si="3"/>
-        <v>4.5100000000000051</v>
-      </c>
-      <c r="O45">
-        <f t="shared" ca="1" si="4"/>
-        <v>3.4400000000000119</v>
-      </c>
-      <c r="P45">
-        <f t="shared" ca="1" si="5"/>
         <v>4.8499999999999943</v>
       </c>
       <c r="R45" s="29">
@@ -4143,7 +4165,7 @@
         <v>0.5</v>
       </c>
       <c r="G46" s="26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>202</v>
       </c>
       <c r="H46" s="22">
@@ -4152,27 +4174,27 @@
       </c>
       <c r="I46" s="24"/>
       <c r="K46">
+        <f t="shared" ca="1" si="7"/>
+        <v>43.3</v>
+      </c>
+      <c r="L46">
+        <f t="shared" ca="1" si="8"/>
+        <v>70</v>
+      </c>
+      <c r="M46">
+        <f t="shared" ca="1" si="9"/>
+        <v>23.5</v>
+      </c>
+      <c r="N46">
+        <f t="shared" ca="1" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="O46">
+        <f t="shared" ca="1" si="5"/>
+        <v>42</v>
+      </c>
+      <c r="P46">
         <f t="shared" ca="1" si="6"/>
-        <v>43.3</v>
-      </c>
-      <c r="L46">
-        <f t="shared" ca="1" si="7"/>
-        <v>70</v>
-      </c>
-      <c r="M46">
-        <f t="shared" ca="1" si="8"/>
-        <v>23.5</v>
-      </c>
-      <c r="N46">
-        <f t="shared" ca="1" si="3"/>
-        <v>32</v>
-      </c>
-      <c r="O46">
-        <f t="shared" ca="1" si="4"/>
-        <v>42</v>
-      </c>
-      <c r="P46">
-        <f t="shared" ca="1" si="5"/>
         <v>49</v>
       </c>
       <c r="R46" s="1"/>
@@ -4188,7 +4210,7 @@
         <v>140</v>
       </c>
       <c r="D47" s="25">
-        <f t="shared" ref="D47:D50" si="16">C47/10</f>
+        <f t="shared" ref="D47:D50" si="17">C47/10</f>
         <v>14</v>
       </c>
       <c r="E47" s="1">
@@ -4198,36 +4220,36 @@
         <v>0.5</v>
       </c>
       <c r="G47" s="26">
-        <f t="shared" ref="G47:G50" si="17">ROUND($C$4/(D47/E47*F47),0)</f>
+        <f t="shared" ref="G47:G50" si="18">ROUND($C$4/(D47/E47*F47),0)</f>
         <v>144</v>
       </c>
       <c r="H47" s="22">
-        <f t="shared" ref="H47:H50" si="18">ROUND(D47/E47,0)</f>
+        <f t="shared" ref="H47:H50" si="19">ROUND(D47/E47,0)</f>
         <v>28</v>
       </c>
       <c r="I47" s="23"/>
       <c r="K47">
+        <f t="shared" ca="1" si="7"/>
+        <v>85.3</v>
+      </c>
+      <c r="L47">
+        <f t="shared" ca="1" si="8"/>
+        <v>85.5</v>
+      </c>
+      <c r="M47">
+        <f t="shared" ca="1" si="9"/>
+        <v>65</v>
+      </c>
+      <c r="N47">
+        <f t="shared" ca="1" si="4"/>
+        <v>65</v>
+      </c>
+      <c r="O47">
+        <f t="shared" ca="1" si="5"/>
+        <v>116</v>
+      </c>
+      <c r="P47">
         <f t="shared" ca="1" si="6"/>
-        <v>85.3</v>
-      </c>
-      <c r="L47">
-        <f t="shared" ca="1" si="7"/>
-        <v>85.5</v>
-      </c>
-      <c r="M47">
-        <f t="shared" ca="1" si="8"/>
-        <v>65</v>
-      </c>
-      <c r="N47">
-        <f t="shared" ca="1" si="3"/>
-        <v>65</v>
-      </c>
-      <c r="O47">
-        <f t="shared" ca="1" si="4"/>
-        <v>116</v>
-      </c>
-      <c r="P47">
-        <f t="shared" ca="1" si="5"/>
         <v>95</v>
       </c>
       <c r="R47" s="1">
@@ -4249,7 +4271,7 @@
         <v>60</v>
       </c>
       <c r="D48" s="25">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>6</v>
       </c>
       <c r="E48" s="1">
@@ -4259,11 +4281,11 @@
         <v>0.5</v>
       </c>
       <c r="G48" s="26">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>34</v>
       </c>
       <c r="H48" s="22">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>120</v>
       </c>
       <c r="I48" s="23"/>
@@ -4284,7 +4306,7 @@
         <v>0.1</v>
       </c>
       <c r="D49" s="25">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.01</v>
       </c>
       <c r="E49" s="22">
@@ -4294,11 +4316,11 @@
         <v>1</v>
       </c>
       <c r="G49" s="26">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>202</v>
       </c>
       <c r="H49" s="22">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>10</v>
       </c>
       <c r="I49" s="24"/>
@@ -4321,7 +4343,7 @@
         <v>550</v>
       </c>
       <c r="D50" s="25">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>55</v>
       </c>
       <c r="E50" s="22">
@@ -4331,11 +4353,11 @@
         <v>1</v>
       </c>
       <c r="G50" s="26">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>37</v>
       </c>
       <c r="H50" s="22">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>55</v>
       </c>
       <c r="I50" s="24"/>
@@ -4356,6 +4378,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>